<commit_message>
new calculations for dh-mrv new formatted statistics files
</commit_message>
<xml_diff>
--- a/src/formatted statistics/1011-fc-2015-10-11-15-23-24.xlsx
+++ b/src/formatted statistics/1011-fc-2015-10-11-15-23-24.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="1011-fc-2015-10-11-15-23-24" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
   <si>
     <t>Heuristics:</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>variance distribution for givens = 29</t>
+  </si>
+  <si>
+    <t>degree_heuristic = False</t>
   </si>
 </sst>
 </file>
@@ -865,11 +868,11 @@
         </c:dLbls>
         <c:gapWidth val="80"/>
         <c:overlap val="25"/>
-        <c:axId val="-461818816"/>
-        <c:axId val="-461817184"/>
+        <c:axId val="1016712448"/>
+        <c:axId val="1016705920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-461818816"/>
+        <c:axId val="1016712448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,7 +915,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-461817184"/>
+        <c:crossAx val="1016705920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -920,7 +923,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-461817184"/>
+        <c:axId val="1016705920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,7 +974,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-461818816"/>
+        <c:crossAx val="1016712448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1180,11 +1183,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-307712224"/>
-        <c:axId val="-307725824"/>
+        <c:axId val="1018693136"/>
+        <c:axId val="1018698576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-307712224"/>
+        <c:axId val="1018693136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,7 +1230,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-307725824"/>
+        <c:crossAx val="1018698576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1235,7 +1238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-307725824"/>
+        <c:axId val="1018698576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1289,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-307712224"/>
+        <c:crossAx val="1018693136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1494,11 +1497,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-454079216"/>
-        <c:axId val="-454089008"/>
+        <c:axId val="1018701296"/>
+        <c:axId val="1018698032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-454079216"/>
+        <c:axId val="1018701296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1555,12 +1558,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-454089008"/>
+        <c:crossAx val="1018698032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-454089008"/>
+        <c:axId val="1018698032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1620,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-454079216"/>
+        <c:crossAx val="1018701296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1825,11 +1828,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-307726368"/>
-        <c:axId val="-307723104"/>
+        <c:axId val="1018702928"/>
+        <c:axId val="1018696400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-307726368"/>
+        <c:axId val="1018702928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1886,12 +1889,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-307723104"/>
+        <c:crossAx val="1018696400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-307723104"/>
+        <c:axId val="1018696400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,7 +1951,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-307726368"/>
+        <c:crossAx val="1018702928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2088,10 +2091,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$35:$A$45</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$35:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.24691358024691301</c:v>
                 </c:pt>
@@ -2099,30 +2102,27 @@
                   <c:v>0.469135802469135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.469135802469135</c:v>
+                  <c:v>0.69135802469135799</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69135802469135799</c:v>
+                  <c:v>0.91358024691357997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.91358024691357997</c:v>
+                  <c:v>1.1358024691358</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1358024691358</c:v>
+                  <c:v>1.3580246913580201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3580246913580201</c:v>
+                  <c:v>1.5802469135802399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5802469135802399</c:v>
+                  <c:v>1.80246913580246</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.80246913580246</c:v>
+                  <c:v>2.0246913580246901</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0246913580246901</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>2.69135802469135</c:v>
                 </c:pt>
               </c:numCache>
@@ -2130,41 +2130,38 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$35:$C$45</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$35:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.54099997878074602</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7262000322341899</c:v>
+                  <c:v>1.2573888831668414</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67137494683265597</c:v>
+                  <c:v>0.78216128964577902</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78216128964577902</c:v>
+                  <c:v>1.0367333412170401</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0367333412170401</c:v>
+                  <c:v>1.04328002929687</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.04328002929687</c:v>
+                  <c:v>4.7015999794006298</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.7015999794006298</c:v>
+                  <c:v>0.32400006055831898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.32400006055831898</c:v>
+                  <c:v>0.466499984264373</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.466499984264373</c:v>
+                  <c:v>0.55750000476837103</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.55750000476837103</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>1.2980000972747801</c:v>
                 </c:pt>
               </c:numCache>
@@ -2180,11 +2177,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-430387040"/>
-        <c:axId val="-430371808"/>
+        <c:axId val="1018699664"/>
+        <c:axId val="1018693680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-430387040"/>
+        <c:axId val="1018699664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,12 +2238,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430371808"/>
+        <c:crossAx val="1018693680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-430371808"/>
+        <c:axId val="1018693680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2303,7 +2300,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430387040"/>
+        <c:crossAx val="1018699664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2443,10 +2440,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$35:$A$45</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$35:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.24691358024691301</c:v>
                 </c:pt>
@@ -2454,30 +2451,27 @@
                   <c:v>0.469135802469135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.469135802469135</c:v>
+                  <c:v>0.69135802469135799</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69135802469135799</c:v>
+                  <c:v>0.91358024691357997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.91358024691357997</c:v>
+                  <c:v>1.1358024691358</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1358024691358</c:v>
+                  <c:v>1.3580246913580201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3580246913580201</c:v>
+                  <c:v>1.5802469135802399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5802469135802399</c:v>
+                  <c:v>1.80246913580246</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.80246913580246</c:v>
+                  <c:v>2.0246913580246901</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0246913580246901</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>2.69135802469135</c:v>
                 </c:pt>
               </c:numCache>
@@ -2485,41 +2479,38 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$35:$D$45</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$35:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>525</c:v>
+                  <c:v>377.88888888888891</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>194</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>226</c:v>
+                  <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>289</c:v>
+                  <c:v>301</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>301</c:v>
+                  <c:v>1287</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1287</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>98</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>154</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>394</c:v>
                 </c:pt>
               </c:numCache>
@@ -2535,11 +2526,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-523611184"/>
-        <c:axId val="-523617712"/>
+        <c:axId val="1019824368"/>
+        <c:axId val="1019826544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-523611184"/>
+        <c:axId val="1019824368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,12 +2587,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-523617712"/>
+        <c:crossAx val="1019826544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-523617712"/>
+        <c:axId val="1019826544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2658,7 +2649,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-523611184"/>
+        <c:crossAx val="1019824368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2763,7 +2754,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$48</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2798,7 +2789,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$49:$A$57</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$48:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2834,7 +2825,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$49:$C$57</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$48:$C$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2878,11 +2869,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-430380512"/>
-        <c:axId val="-430372896"/>
+        <c:axId val="1019829264"/>
+        <c:axId val="1019826000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-430380512"/>
+        <c:axId val="1019829264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2939,12 +2930,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430372896"/>
+        <c:crossAx val="1019826000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-430372896"/>
+        <c:axId val="1019826000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3001,7 +2992,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430380512"/>
+        <c:crossAx val="1019829264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3106,7 +3097,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$48</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3141,7 +3132,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$49:$A$57</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$48:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3177,7 +3168,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$49:$D$57</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$48:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3221,11 +3212,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-530726432"/>
-        <c:axId val="-530713920"/>
+        <c:axId val="1019828720"/>
+        <c:axId val="1019829808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-530726432"/>
+        <c:axId val="1019828720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3282,12 +3273,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-530713920"/>
+        <c:crossAx val="1019829808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-530713920"/>
+        <c:axId val="1019829808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3344,7 +3335,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-530726432"/>
+        <c:crossAx val="1019828720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3459,7 +3450,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$60</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3494,7 +3485,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$61:$A$73</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$60:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3542,7 +3533,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$61:$C$73</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$60:$C$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3598,11 +3589,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-423936592"/>
-        <c:axId val="-423929520"/>
+        <c:axId val="1019831440"/>
+        <c:axId val="1019820016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-423936592"/>
+        <c:axId val="1019831440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3659,12 +3650,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423929520"/>
+        <c:crossAx val="1019820016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-423929520"/>
+        <c:axId val="1019820016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3721,7 +3712,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423936592"/>
+        <c:crossAx val="1019831440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3826,7 +3817,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$60</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3861,7 +3852,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$61:$A$73</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$60:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3909,7 +3900,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$61:$D$73</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$60:$D$72</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3965,11 +3956,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-430382688"/>
-        <c:axId val="-430386496"/>
+        <c:axId val="1019821104"/>
+        <c:axId val="1019820560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-430382688"/>
+        <c:axId val="1019821104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4026,12 +4017,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430386496"/>
+        <c:crossAx val="1019820560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-430386496"/>
+        <c:axId val="1019820560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4088,7 +4079,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430382688"/>
+        <c:crossAx val="1019821104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4193,7 +4184,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$76</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4228,7 +4219,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$77:$A$88</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$76:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4273,7 +4264,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$77:$C$88</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$76:$C$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4326,11 +4317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-307714400"/>
-        <c:axId val="-307731808"/>
+        <c:axId val="1019821648"/>
+        <c:axId val="1019819472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-307714400"/>
+        <c:axId val="1019821648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4387,12 +4378,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-307731808"/>
+        <c:crossAx val="1019819472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-307731808"/>
+        <c:axId val="1019819472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4449,7 +4440,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-307714400"/>
+        <c:crossAx val="1019821648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4647,11 +4638,11 @@
         </c:dLbls>
         <c:gapWidth val="80"/>
         <c:overlap val="25"/>
-        <c:axId val="-430378336"/>
-        <c:axId val="-430375072"/>
+        <c:axId val="1016717344"/>
+        <c:axId val="1016717888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-430378336"/>
+        <c:axId val="1016717344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4750,7 +4741,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430375072"/>
+        <c:crossAx val="1016717888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4758,7 +4749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-430375072"/>
+        <c:axId val="1016717888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4809,7 +4800,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430378336"/>
+        <c:crossAx val="1016717344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4914,7 +4905,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$76</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4949,7 +4940,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$77:$A$88</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$76:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4994,7 +4985,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$77:$D$88</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$76:$D$87</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5047,11 +5038,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-461819904"/>
-        <c:axId val="-461815008"/>
+        <c:axId val="1019818384"/>
+        <c:axId val="1019818928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-461819904"/>
+        <c:axId val="1019818384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5108,12 +5099,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-461815008"/>
+        <c:crossAx val="1019818928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-461815008"/>
+        <c:axId val="1019818928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5170,7 +5161,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-461819904"/>
+        <c:crossAx val="1019818384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5275,7 +5266,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$91</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5310,7 +5301,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$92:$A$103</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$91:$A$102</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5355,7 +5346,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$92:$C$103</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$91:$C$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5408,11 +5399,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-523616624"/>
-        <c:axId val="-523607376"/>
+        <c:axId val="1019823824"/>
+        <c:axId val="1019726784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-523616624"/>
+        <c:axId val="1019823824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5469,12 +5460,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-523607376"/>
+        <c:crossAx val="1019726784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-523607376"/>
+        <c:axId val="1019726784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5531,7 +5522,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-523616624"/>
+        <c:crossAx val="1019823824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5628,124 +5619,114 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$91</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$105</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>average splits</c:v>
+                  <c:v>average runtime</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$92:$A$103</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$106:$A$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.44444444444444398</c:v>
+                  <c:v>0.32098765432098703</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66666666666666596</c:v>
+                  <c:v>0.76543209876543195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88888888888888795</c:v>
+                  <c:v>0.98765432098765404</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1111111111111101</c:v>
+                  <c:v>1.2098765432098699</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3333333333333299</c:v>
+                  <c:v>1.43209876543209</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.55555555555555</c:v>
+                  <c:v>1.6543209876543199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7777777777777699</c:v>
+                  <c:v>2.0987654320987601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.2222222222222201</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.4444444444444402</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.6666666666666599</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.88888888888888</c:v>
+                  <c:v>2.3209876543209802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$92:$D$103</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$106:$C$113</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>84</c:v>
+                  <c:v>0.12700009346008301</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>7.2999954223632799E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65</c:v>
+                  <c:v>5.9000015258789E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93</c:v>
+                  <c:v>0.12640004158019999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>109</c:v>
+                  <c:v>1.27600002288818</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>4.3999910354614202E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>171</c:v>
+                  <c:v>0.18950009346008301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>171</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>35</c:v>
+                  <c:v>0.10950005054473801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5755,18 +5736,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-788127824"/>
-        <c:axId val="-788127280"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-788127824"/>
+        <c:axId val="1019733312"/>
+        <c:axId val="1019724608"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1019733312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5776,8 +5769,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -5804,15 +5797,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-788127280"/>
+        <c:crossAx val="1019724608"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="-788127280"/>
+        <c:axId val="1019724608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5832,14 +5822,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -5863,9 +5859,9 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-788127824"/>
+        <c:crossAx val="1019733312"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5968,11 +5964,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$106</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$105</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>average runtime</c:v>
+                  <c:v>average splits</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6003,7 +5999,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$107:$A$114</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$106:$A$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6036,33 +6032,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$C$107:$C$114</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$106:$D$113</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.12700009346008301</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2999954223632799E-2</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9000015258789E-2</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12640004158019999</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.27600002288818</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3999910354614202E-2</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.18950009346008301</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10950005054473801</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6077,11 +6073,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-307705152"/>
-        <c:axId val="-307719840"/>
+        <c:axId val="1019728416"/>
+        <c:axId val="1019739296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-307705152"/>
+        <c:axId val="1019728416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6138,12 +6134,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-307719840"/>
+        <c:crossAx val="1019739296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-307719840"/>
+        <c:axId val="1019739296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6163,7 +6159,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6200,7 +6196,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-307705152"/>
+        <c:crossAx val="1019728416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6305,7 +6301,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$106</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6340,66 +6336,90 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$107:$A$114</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$91:$A$102</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.32098765432098703</c:v>
+                  <c:v>0.44444444444444398</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76543209876543195</c:v>
+                  <c:v>0.66666666666666596</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98765432098765404</c:v>
+                  <c:v>0.88888888888888795</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2098765432098699</c:v>
+                  <c:v>1.1111111111111101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.43209876543209</c:v>
+                  <c:v>1.3333333333333299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6543209876543199</c:v>
+                  <c:v>1.55555555555555</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0987654320987601</c:v>
+                  <c:v>1.7777777777777699</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3209876543209802</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2222222222222201</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4444444444444402</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6666666666666599</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.88888888888888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$107:$D$114</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$91:$D$102</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>349</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6414,11 +6434,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-430382144"/>
-        <c:axId val="-430379968"/>
+        <c:axId val="1125446416"/>
+        <c:axId val="1125447504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-430382144"/>
+        <c:axId val="1125446416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6475,12 +6495,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430379968"/>
+        <c:crossAx val="1125447504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-430379968"/>
+        <c:axId val="1125447504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6537,7 +6557,344 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-430382144"/>
+        <c:crossAx val="1125446416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>average splits</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$60:$A$67</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.172839506172839</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39506172839506098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61728395061728303</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83950617283950602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.06172839506172</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2839506172839501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.50617283950617</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7283950617283901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$D$60:$D$67</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>391</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="854395552"/>
+        <c:axId val="854394464"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="854395552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="854394464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="854394464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="854395552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6664,10 +7021,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$35:$A$45</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$35:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.24691358024691301</c:v>
                 </c:pt>
@@ -6675,30 +7032,27 @@
                   <c:v>0.469135802469135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.469135802469135</c:v>
+                  <c:v>0.69135802469135799</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69135802469135799</c:v>
+                  <c:v>0.91358024691357997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.91358024691357997</c:v>
+                  <c:v>1.1358024691358</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1358024691358</c:v>
+                  <c:v>1.3580246913580201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3580246913580201</c:v>
+                  <c:v>1.5802469135802399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5802469135802399</c:v>
+                  <c:v>1.80246913580246</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.80246913580246</c:v>
+                  <c:v>2.0246913580246901</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0246913580246901</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>2.69135802469135</c:v>
                 </c:pt>
               </c:numCache>
@@ -6706,10 +7060,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$35:$B$45</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$35:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -6717,30 +7071,27 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -6757,11 +7108,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-423920272"/>
-        <c:axId val="-423928432"/>
+        <c:axId val="1016708640"/>
+        <c:axId val="1016714624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-423920272"/>
+        <c:axId val="1016708640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6860,7 +7211,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423928432"/>
+        <c:crossAx val="1016714624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6868,7 +7219,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-423928432"/>
+        <c:axId val="1016714624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6919,7 +7270,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423920272"/>
+        <c:crossAx val="1016708640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7025,7 +7376,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$48</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7046,7 +7397,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$49:$A$57</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$48:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -7082,7 +7433,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$49:$B$57</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$48:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -7127,11 +7478,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-423916464"/>
-        <c:axId val="-423915920"/>
+        <c:axId val="1016707552"/>
+        <c:axId val="1016715168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-423916464"/>
+        <c:axId val="1016707552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7230,7 +7581,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423915920"/>
+        <c:crossAx val="1016715168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7238,7 +7589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-423915920"/>
+        <c:axId val="1016715168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7289,7 +7640,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423916464"/>
+        <c:crossAx val="1016707552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7395,7 +7746,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$60</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7416,7 +7767,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$61:$A$73</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$60:$A$72</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
@@ -7464,7 +7815,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$61:$B$73</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$60:$B$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -7521,11 +7872,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-424723920"/>
-        <c:axId val="-424722832"/>
+        <c:axId val="1016716800"/>
+        <c:axId val="1016706464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-424723920"/>
+        <c:axId val="1016716800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7568,7 +7919,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-424722832"/>
+        <c:crossAx val="1016706464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7576,7 +7927,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-424722832"/>
+        <c:axId val="1016706464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7627,7 +7978,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-424723920"/>
+        <c:crossAx val="1016716800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7733,7 +8084,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$76</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7754,7 +8105,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$77:$A$88</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$76:$A$87</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -7799,7 +8150,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$77:$B$88</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$76:$B$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -7853,11 +8204,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-423936048"/>
-        <c:axId val="-423933872"/>
+        <c:axId val="1016709728"/>
+        <c:axId val="1016707008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-423936048"/>
+        <c:axId val="1016709728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7956,7 +8307,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423933872"/>
+        <c:crossAx val="1016707008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7964,7 +8315,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-423933872"/>
+        <c:axId val="1016707008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8015,7 +8366,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423936048"/>
+        <c:crossAx val="1016709728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8121,7 +8472,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$91</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8142,7 +8493,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$92:$A$103</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$91:$A$102</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -8187,7 +8538,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$92:$B$103</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$91:$B$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -8241,11 +8592,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-424720112"/>
-        <c:axId val="-424719568"/>
+        <c:axId val="1018689328"/>
+        <c:axId val="1018695312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-424720112"/>
+        <c:axId val="1018689328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8344,7 +8695,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-424719568"/>
+        <c:crossAx val="1018695312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8352,7 +8703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-424719568"/>
+        <c:axId val="1018695312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8403,7 +8754,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-424720112"/>
+        <c:crossAx val="1018689328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8509,7 +8860,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$106</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$105</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8530,7 +8881,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$107:$A$114</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$A$106:$A$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8563,7 +8914,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$107:$B$114</c:f>
+              <c:f>'1011-fc-2015-10-11-15-23-24'!$B$106:$B$113</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8605,11 +8956,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-431298368"/>
-        <c:axId val="-431305440"/>
+        <c:axId val="1018690416"/>
+        <c:axId val="1018694768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-431298368"/>
+        <c:axId val="1018690416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8708,7 +9059,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-431305440"/>
+        <c:crossAx val="1018694768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8716,7 +9067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-431305440"/>
+        <c:axId val="1018694768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8767,7 +9118,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-431298368"/>
+        <c:crossAx val="1018690416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8976,11 +9327,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-423932240"/>
-        <c:axId val="-423931696"/>
+        <c:axId val="1018692048"/>
+        <c:axId val="1018691504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-423932240"/>
+        <c:axId val="1018692048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9023,7 +9374,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423931696"/>
+        <c:crossAx val="1018691504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9031,7 +9382,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-423931696"/>
+        <c:axId val="1018691504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9082,7 +9433,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-423932240"/>
+        <c:crossAx val="1018692048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9811,6 +10162,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors25.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17268,7 +17659,7 @@
 </file>
 
 <file path=xl/charts/style22.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -17295,8 +17686,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -17397,7 +17788,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -17429,10 +17820,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -17472,22 +17863,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -17592,8 +17984,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -17725,19 +18117,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -17751,6 +18144,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -18287,6 +18691,522 @@
 </file>
 
 <file path=xl/charts/style24.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style25.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -22408,7 +23328,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>162877</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22432,13 +23352,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>319087</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22462,13 +23382,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>357187</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>71436</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22492,13 +23412,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>414337</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>109537</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22522,13 +23442,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>280987</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>585787</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22552,13 +23472,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>252412</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>464343</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>121312</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22708,7 +23628,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>5953</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22738,7 +23658,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>72627</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22762,13 +23682,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>321469</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>59530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>252016</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>91677</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22790,16 +23710,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>345281</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>3571</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>321469</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>182165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>59531</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>79771</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>35719</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>67865</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22822,13 +23742,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>95251</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>15477</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>416719</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22852,13 +23772,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>500062</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>39290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>115490</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22882,13 +23802,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>75009</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>511968</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>151209</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22912,13 +23832,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>107157</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>86915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>163115</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22942,13 +23862,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>130969</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>98822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>452437</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>175022</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22970,20 +23890,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>35718</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>63102</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>226219</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>27384</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>357186</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>139302</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>103584</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="26" name="Chart 25"/>
+        <xdr:cNvPr id="27" name="Chart 26"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -23000,20 +23920,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>226219</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>27384</xdr:rowOff>
+      <xdr:rowOff>63103</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>345281</xdr:colOff>
       <xdr:row>119</xdr:row>
-      <xdr:rowOff>103584</xdr:rowOff>
+      <xdr:rowOff>139303</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="27" name="Chart 26"/>
+        <xdr:cNvPr id="28" name="Chart 27"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -23030,20 +23950,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>23813</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>63103</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>345281</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>139303</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="28" name="Chart 27"/>
+        <xdr:cNvPr id="9" name="Chart 8"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -23053,6 +23973,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>363144</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>11907</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>35721</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>79772</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -23324,10 +24274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23335,7 +24285,7 @@
     <col min="1" max="1" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" customWidth="1"/>
     <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -23348,6 +24298,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -23743,1073 +24696,1061 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>1.7262000322341899</v>
+        <f xml:space="preserve"> ( 10 * 1.72620003223419 + 8 * 0.671374946832656) / 18</f>
+        <v>1.2573888831668414</v>
       </c>
       <c r="D36" s="2">
-        <v>525</v>
+        <f xml:space="preserve"> ( 10 * 525 + 8 * 194) / 18</f>
+        <v>377.88888888888891</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>0.469135802469135</v>
+        <v>0.69135802469135799</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C37">
-        <v>0.67137494683265597</v>
+        <v>0.78216128964577902</v>
       </c>
       <c r="D37" s="2">
-        <v>194</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>0.69135802469135799</v>
+        <v>0.91358024691357997</v>
       </c>
       <c r="B38">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C38">
-        <v>0.78216128964577902</v>
+        <v>1.0367333412170401</v>
       </c>
       <c r="D38" s="2">
-        <v>226</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>0.91358024691357997</v>
+        <v>1.1358024691358</v>
       </c>
       <c r="B39">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C39">
-        <v>1.0367333412170401</v>
+        <v>1.04328002929687</v>
       </c>
       <c r="D39" s="2">
-        <v>289</v>
+        <v>301</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>1.1358024691358</v>
+        <v>1.3580246913580201</v>
       </c>
       <c r="B40">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C40">
-        <v>1.04328002929687</v>
+        <v>4.7015999794006298</v>
       </c>
       <c r="D40" s="2">
-        <v>301</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>1.3580246913580201</v>
+        <v>1.5802469135802399</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>4.7015999794006298</v>
+        <v>0.32400006055831898</v>
       </c>
       <c r="D41" s="2">
-        <v>1287</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>1.5802469135802399</v>
+        <v>1.80246913580246</v>
       </c>
       <c r="B42">
         <v>4</v>
       </c>
       <c r="C42">
-        <v>0.32400006055831898</v>
+        <v>0.466499984264373</v>
       </c>
       <c r="D42" s="2">
-        <v>98</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>1.80246913580246</v>
+        <v>2.0246913580246901</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C43">
-        <v>0.466499984264373</v>
+        <v>0.55750000476837103</v>
       </c>
       <c r="D43" s="2">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>2.0246913580246901</v>
+        <v>2.69135802469135</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>0.55750000476837103</v>
+        <v>1.2980000972747801</v>
       </c>
       <c r="D44" s="2">
-        <v>162</v>
+        <v>394</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>2.69135802469135</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>1.2980000972747801</v>
-      </c>
-      <c r="D45" s="2">
-        <v>394</v>
+      <c r="A45" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>10</v>
+      <c r="A48" s="1">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>0.41863627867265102</v>
+      </c>
+      <c r="D48" s="2">
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>0.22222222222222199</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="B49">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C49">
-        <v>0.41863627867265102</v>
+        <v>0.457758615756857</v>
       </c>
       <c r="D49" s="2">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>0.44444444444444398</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="B50">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C50">
-        <v>0.457758615756857</v>
+        <v>0.72653489334638699</v>
       </c>
       <c r="D50" s="2">
-        <v>133</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>0.66666666666666596</v>
+        <v>0.88888888888888795</v>
       </c>
       <c r="B51">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C51">
-        <v>0.72653489334638699</v>
+        <v>1.1934558889445099</v>
       </c>
       <c r="D51" s="2">
-        <v>216</v>
+        <v>347</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>0.88888888888888795</v>
+        <v>1.1111111111111101</v>
       </c>
       <c r="B52">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C52">
-        <v>1.1934558889445099</v>
+        <v>0.77135296428904798</v>
       </c>
       <c r="D52" s="2">
-        <v>347</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>1.1111111111111101</v>
+        <v>1.3333333333333299</v>
       </c>
       <c r="B53">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C53">
-        <v>0.77135296428904798</v>
+        <v>1.7232749998569401</v>
       </c>
       <c r="D53" s="2">
-        <v>224</v>
+        <v>518</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>1.3333333333333299</v>
+        <v>1.55555555555555</v>
       </c>
       <c r="B54">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C54">
-        <v>1.7232749998569401</v>
+        <v>1.6766500592231699</v>
       </c>
       <c r="D54" s="2">
-        <v>518</v>
+        <v>478</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>1.55555555555555</v>
+        <v>1.7777777777777699</v>
       </c>
       <c r="B55">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C55">
-        <v>1.6766500592231699</v>
+        <v>1.2771111329396501</v>
       </c>
       <c r="D55" s="2">
-        <v>478</v>
+        <v>365</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>1.7777777777777699</v>
+        <v>2</v>
       </c>
       <c r="B56">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C56">
-        <v>1.2771111329396501</v>
+        <v>1.2879999478658</v>
       </c>
       <c r="D56" s="2">
-        <v>365</v>
+        <v>388</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>2</v>
-      </c>
-      <c r="B57">
+      <c r="A57" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C57">
-        <v>1.2879999478658</v>
-      </c>
-      <c r="D57" s="2">
-        <v>388</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>10</v>
+      <c r="A60" s="1">
+        <v>0.172839506172839</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>0.26266662279764802</v>
+      </c>
+      <c r="D60" s="2">
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>0.172839506172839</v>
+        <v>0.39506172839506098</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C61">
-        <v>0.26266662279764802</v>
+        <v>0.205375015735626</v>
       </c>
       <c r="D61" s="2">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>0.39506172839506098</v>
+        <v>0.61728395061728303</v>
       </c>
       <c r="B62">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C62">
-        <v>0.205375015735626</v>
+        <v>0.517949998378753</v>
       </c>
       <c r="D62" s="2">
-        <v>59</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>0.61728395061728303</v>
+        <v>0.83950617283950602</v>
       </c>
       <c r="B63">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C63">
-        <v>0.517949998378753</v>
+        <v>0.27641178579891401</v>
       </c>
       <c r="D63" s="2">
-        <v>154</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>0.83950617283950602</v>
+        <v>1.06172839506172</v>
       </c>
       <c r="B64">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C64">
-        <v>0.27641178579891401</v>
+        <v>0.501022222306993</v>
       </c>
       <c r="D64" s="2">
-        <v>81</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>1.06172839506172</v>
+        <v>1.2839506172839501</v>
       </c>
       <c r="B65">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C65">
-        <v>0.501022222306993</v>
+        <f>(26*0.411961537141066+24* 0.703880004882812)/50</f>
+        <v>0.55208240165710409</v>
       </c>
       <c r="D65" s="2">
-        <v>146</v>
+        <f>(26 * 115 + 24 * 206) /50</f>
+        <v>158.68</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>1.2839506172839501</v>
+        <v>1.50617283950617</v>
       </c>
       <c r="B66">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C66">
-        <f>(26*0.411961537141066+24* 0.703880004882812)/50</f>
-        <v>0.55208240165710409</v>
+        <v>0.60220831632614102</v>
       </c>
       <c r="D66" s="2">
-        <f>(26 * 115 + 24 * 206) /50</f>
-        <v>158.68</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>1.50617283950617</v>
+        <v>1.7283950617283901</v>
       </c>
       <c r="B67">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C67">
-        <v>0.60220831632614102</v>
+        <v>1.48841179118436</v>
       </c>
       <c r="D67" s="2">
-        <v>171</v>
+        <v>391</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>1.7283950617283901</v>
+        <v>1.95061728395061</v>
       </c>
       <c r="B68">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C68">
-        <v>1.48841179118436</v>
+        <v>0.41027274998751501</v>
       </c>
       <c r="D68" s="2">
-        <v>391</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>1.95061728395061</v>
+        <v>2.1728395061728301</v>
       </c>
       <c r="B69">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C69">
-        <v>0.41027274998751501</v>
+        <f xml:space="preserve"> (3 * 4.50600004196166 + 4* 0.325749993324279) /7</f>
+        <v>2.1172857284545854</v>
       </c>
       <c r="D69" s="2">
-        <v>121</v>
+        <f>(3 * 1309 + 4 * 97) /7</f>
+        <v>616.42857142857144</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>2.1728395061728301</v>
+        <v>2.3950617283950599</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C70">
-        <f xml:space="preserve"> (3 * 4.50600004196166 + 4* 0.325749993324279) /7</f>
-        <v>2.1172857284545854</v>
+        <v>7.2415000200271598</v>
       </c>
       <c r="D70" s="2">
-        <f>(3 * 1309 + 4 * 97) /7</f>
-        <v>616.42857142857144</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>2.3950617283950599</v>
+        <v>2.61728395061728</v>
       </c>
       <c r="B71">
         <v>2</v>
       </c>
       <c r="C71">
-        <v>7.2415000200271598</v>
+        <v>4.7404999732971103</v>
       </c>
       <c r="D71" s="2">
-        <v>2111</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>2.61728395061728</v>
+        <v>2.8395061728395001</v>
       </c>
       <c r="B72">
         <v>2</v>
       </c>
       <c r="C72">
-        <v>4.7404999732971103</v>
+        <v>0.69050002098083496</v>
       </c>
       <c r="D72" s="2">
-        <v>1397</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>2.8395061728395001</v>
-      </c>
-      <c r="B73">
-        <v>2</v>
-      </c>
-      <c r="C73">
-        <v>0.69050002098083496</v>
-      </c>
-      <c r="D73" s="2">
-        <v>220</v>
+      <c r="A73" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B76" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" t="s">
-        <v>9</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>10</v>
+      <c r="A76" s="1">
+        <v>0.32098765432098703</v>
+      </c>
+      <c r="B76">
+        <v>4</v>
+      </c>
+      <c r="C76">
+        <v>7.0249974727630601E-2</v>
+      </c>
+      <c r="D76" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>0.32098765432098703</v>
+        <v>0.54320987654320996</v>
       </c>
       <c r="B77">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C77">
-        <v>7.0249974727630601E-2</v>
+        <v>0.173655172874187</v>
       </c>
       <c r="D77" s="2">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>0.54320987654320996</v>
+        <v>0.76543209876543195</v>
       </c>
       <c r="B78">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C78">
-        <v>0.173655172874187</v>
+        <v>0.243041684230168</v>
       </c>
       <c r="D78" s="2">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>0.76543209876543195</v>
+        <v>0.98765432098765404</v>
       </c>
       <c r="B79">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C79">
-        <v>0.243041684230168</v>
+        <v>0.51423683919404595</v>
       </c>
       <c r="D79" s="2">
-        <v>71</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>0.98765432098765404</v>
+        <v>1.2098765432098699</v>
       </c>
       <c r="B80">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C80">
-        <v>0.51423683919404595</v>
+        <v>0.35709758502680999</v>
       </c>
       <c r="D80" s="2">
-        <v>148</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>1.2098765432098699</v>
+        <v>1.43209876543209</v>
       </c>
       <c r="B81">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C81">
-        <v>0.35709758502680999</v>
+        <v>0.22820833325386</v>
       </c>
       <c r="D81" s="2">
-        <v>100</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>1.43209876543209</v>
+        <v>1.6543209876543199</v>
       </c>
       <c r="B82">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C82">
-        <v>0.22820833325386</v>
+        <v>0.39469999074935902</v>
       </c>
       <c r="D82" s="2">
-        <v>65</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>1.6543209876543199</v>
+        <v>1.87654320987654</v>
       </c>
       <c r="B83">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C83">
-        <v>0.39469999074935902</v>
+        <v>1.46041665474573</v>
       </c>
       <c r="D83" s="2">
-        <v>114</v>
+        <v>396</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>1.87654320987654</v>
+        <v>2.0987654320987601</v>
       </c>
       <c r="B84">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C84">
-        <v>1.46041665474573</v>
+        <v>0.331599950790405</v>
       </c>
       <c r="D84" s="2">
-        <v>396</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>2.0987654320987601</v>
+        <v>2.3209876543209802</v>
       </c>
       <c r="B85">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C85">
-        <v>0.331599950790405</v>
+        <f xml:space="preserve"> (0.290999889373779 + 0.00999999046325683) /2</f>
+        <v>0.15049993991851793</v>
       </c>
       <c r="D85" s="2">
-        <v>98</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>2.3209876543209802</v>
+        <v>2.5432098765431999</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C86">
-        <f xml:space="preserve"> (0.290999889373779 + 0.00999999046325683) /2</f>
-        <v>0.15049993991851793</v>
+        <v>4.6499967575073201E-2</v>
       </c>
       <c r="D86" s="2">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>2.5432098765431999</v>
+        <v>2.7654320987654302</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C87">
-        <v>4.6499967575073201E-2</v>
+        <v>0.12299990653991601</v>
       </c>
       <c r="D87" s="2">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>2.7654320987654302</v>
-      </c>
-      <c r="B88">
-        <v>1</v>
-      </c>
-      <c r="C88">
-        <v>0.12299990653991601</v>
-      </c>
-      <c r="D88" s="2">
-        <v>40</v>
+      <c r="A88" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B91" t="s">
-        <v>8</v>
-      </c>
-      <c r="C91" t="s">
-        <v>9</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>10</v>
+      <c r="A91" s="1">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="B91">
+        <v>6</v>
+      </c>
+      <c r="C91">
+        <v>0.29233332475026402</v>
+      </c>
+      <c r="D91" s="2">
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>0.44444444444444398</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="B92">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C92">
-        <v>0.29233332475026402</v>
+        <v>6.4500033855438205E-2</v>
       </c>
       <c r="D92" s="2">
-        <v>84</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>0.66666666666666596</v>
+        <v>0.88888888888888795</v>
       </c>
       <c r="B93">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C93">
-        <v>6.4500033855438205E-2</v>
+        <v>0.202384636952326</v>
       </c>
       <c r="D93" s="2">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>0.88888888888888795</v>
+        <v>1.1111111111111101</v>
       </c>
       <c r="B94">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C94">
-        <v>0.202384636952326</v>
+        <v>0.30758339166641202</v>
       </c>
       <c r="D94" s="2">
-        <v>65</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>1.1111111111111101</v>
+        <v>1.3333333333333299</v>
       </c>
       <c r="B95">
         <v>12</v>
       </c>
       <c r="C95">
-        <v>0.30758339166641202</v>
+        <v>0.36183329423268601</v>
       </c>
       <c r="D95" s="2">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>1.3333333333333299</v>
+        <v>1.55555555555555</v>
       </c>
       <c r="B96">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C96">
-        <v>0.36183329423268601</v>
+        <v>7.8999962125505696E-2</v>
       </c>
       <c r="D96" s="2">
-        <v>109</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>1.55555555555555</v>
+        <v>1.7777777777777699</v>
       </c>
       <c r="B97">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C97">
-        <v>7.8999962125505696E-2</v>
+        <v>0.55099999904632502</v>
       </c>
       <c r="D97" s="2">
-        <v>24</v>
+        <v>171</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>1.7777777777777699</v>
+        <v>2</v>
       </c>
       <c r="B98">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C98">
-        <v>0.55099999904632502</v>
+        <v>0.19133334689670101</v>
       </c>
       <c r="D98" s="2">
-        <v>171</v>
+        <v>59</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>2</v>
+        <v>2.2222222222222201</v>
       </c>
       <c r="B99">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C99">
-        <v>0.19133334689670101</v>
+        <v>0.170249938964843</v>
       </c>
       <c r="D99" s="2">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>2.2222222222222201</v>
+        <v>2.4444444444444402</v>
       </c>
       <c r="B100">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C100">
-        <v>0.170249938964843</v>
+        <v>0.47399997711181602</v>
       </c>
       <c r="D100" s="2">
-        <v>52</v>
+        <v>171</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>2.4444444444444402</v>
+        <v>2.6666666666666599</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C101">
-        <v>0.47399997711181602</v>
+        <v>0.10899996757507301</v>
       </c>
       <c r="D101" s="2">
-        <v>171</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>2.6666666666666599</v>
+        <v>2.88888888888888</v>
       </c>
       <c r="B102">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C102">
-        <v>0.10899996757507301</v>
+        <v>9.4333410263061496E-2</v>
       </c>
       <c r="D102" s="2">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>2.88888888888888</v>
-      </c>
-      <c r="B103">
+      <c r="A103" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C103">
-        <v>9.4333410263061496E-2</v>
-      </c>
-      <c r="D103" s="2">
-        <v>35</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="B105" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B106" t="s">
-        <v>8</v>
-      </c>
-      <c r="C106" t="s">
-        <v>9</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>10</v>
+      <c r="A106" s="1">
+        <v>0.32098765432098703</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>0.12700009346008301</v>
+      </c>
+      <c r="D106" s="2">
+        <v>36</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>0.32098765432098703</v>
+        <v>0.76543209876543195</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
       <c r="C107">
-        <v>0.12700009346008301</v>
+        <v>7.2999954223632799E-2</v>
       </c>
       <c r="D107" s="2">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>0.76543209876543195</v>
+        <v>0.98765432098765404</v>
       </c>
       <c r="B108">
         <v>1</v>
       </c>
       <c r="C108">
-        <v>7.2999954223632799E-2</v>
+        <v>5.9000015258789E-2</v>
       </c>
       <c r="D108" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>0.98765432098765404</v>
+        <v>1.2098765432098699</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C109">
-        <v>5.9000015258789E-2</v>
+        <v>0.12640004158019999</v>
       </c>
       <c r="D109" s="2">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>1.2098765432098699</v>
+        <v>1.43209876543209</v>
       </c>
       <c r="B110">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C110">
-        <v>0.12640004158019999</v>
+        <v>1.27600002288818</v>
       </c>
       <c r="D110" s="2">
-        <v>41</v>
+        <v>349</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>1.43209876543209</v>
+        <v>1.6543209876543199</v>
       </c>
       <c r="B111">
         <v>1</v>
       </c>
       <c r="C111">
-        <v>1.27600002288818</v>
+        <v>4.3999910354614202E-2</v>
       </c>
       <c r="D111" s="2">
-        <v>349</v>
+        <v>15</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>1.6543209876543199</v>
+        <v>2.0987654320987601</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C112">
-        <v>4.3999910354614202E-2</v>
+        <v>0.18950009346008301</v>
       </c>
       <c r="D112" s="2">
-        <v>15</v>
+        <v>62</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>2.0987654320987601</v>
+        <v>2.3209876543209802</v>
       </c>
       <c r="B113">
         <v>2</v>
       </c>
       <c r="C113">
-        <v>0.18950009346008301</v>
+        <v>0.10950005054473801</v>
       </c>
       <c r="D113" s="2">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <v>2.3209876543209802</v>
-      </c>
-      <c r="B114">
-        <v>2</v>
-      </c>
-      <c r="C114">
-        <v>0.10950005054473801</v>
-      </c>
-      <c r="D114" s="2">
-        <v>39</v>
+      <c r="A114" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="B116" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" t="s">
+        <v>9</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B117" t="s">
-        <v>8</v>
-      </c>
-      <c r="C117" t="s">
-        <v>9</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>10</v>
+      <c r="A117" s="1">
+        <v>1.2839506172839501</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117">
+        <v>0.14499998092651301</v>
+      </c>
+      <c r="D117" s="2">
+        <v>46</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>1.2839506172839501</v>
+        <v>2.61728395061728</v>
       </c>
       <c r="B118">
         <v>1</v>
       </c>
       <c r="C118">
-        <v>0.14499998092651301</v>
+        <v>4.9999952316284103E-2</v>
       </c>
       <c r="D118" s="2">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>2.61728395061728</v>
-      </c>
-      <c r="B119">
-        <v>1</v>
-      </c>
-      <c r="C119">
-        <v>4.9999952316284103E-2</v>
-      </c>
-      <c r="D119" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="A119" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>